<commit_message>
fix in recode.others function
fix in recode.others function

fix
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/res_elsewhere.xlsx
+++ b/tests/testthat/fixtures/res_elsewhere.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve">uuid</t>
   </si>
@@ -59,40 +59,34 @@
     <t xml:space="preserve">ddcb5d94-f187-45ea-92c2-4f29a9909be4</t>
   </si>
   <si>
-    <t xml:space="preserve">a7_site_management_receive_compensation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no_compensation other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no_compensation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a7_site_management_receive_compensation/other</t>
+    <t xml:space="preserve">a7_1_site_management_receive_compensation_other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">myother;Phone Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">myother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a9_2_organization_provided_assistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">humanitarian_agency other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">humanitarian_agency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recode elsewhere other;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a9_2_organization_provided_assistance/other</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a7_1_site_management_receive_compensation_other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a9_2_organization_provided_assistance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">humanitarian_agency other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">humanitarian_agency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a9_2_organization_provided_assistance/other</t>
   </si>
   <si>
     <t xml:space="preserve">a9_2_1_organization_provided_assistance_other</t>
@@ -540,10 +534,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
@@ -556,26 +550,28 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
         <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6"/>
-      <c r="G6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -587,52 +583,48 @@
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F7"/>
       <c r="G7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F8"/>
       <c r="G8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="s">
@@ -641,17 +633,17 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="s">
@@ -660,17 +652,17 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="s">
@@ -679,17 +671,17 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="s">
         <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F12"/>
       <c r="G12" t="s">
@@ -698,17 +690,17 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13"/>
       <c r="D13" t="s">
         <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="s">
@@ -717,17 +709,17 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="s">
@@ -736,17 +728,17 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="s">
@@ -755,58 +747,20 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
         <v>34</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
       </c>
       <c r="F16"/>
       <c r="G16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17"/>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17"/>
-      <c r="G17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18"/>
-      <c r="D18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18"/>
-      <c r="G18" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>